<commit_message>
diletation erosion grecon result
</commit_message>
<xml_diff>
--- a/data/vysledky-mazani.xlsx
+++ b/data/vysledky-mazani.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\bakalarska-prace\bakalarska-prace\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E3CDC9-29C1-4AF6-A0E9-2D4690CF9B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA13811-4679-4DE0-9C3D-F52784E0D360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3CC789BC-E248-4C1E-B58B-9660197E393A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>dataset</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>0.35</t>
+  </si>
+  <si>
+    <t>diletation - erosion</t>
+  </si>
+  <si>
+    <t>3x3 unit</t>
   </si>
 </sst>
 </file>
@@ -139,7 +145,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -410,11 +416,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -431,16 +466,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
@@ -451,11 +480,37 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="17">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
@@ -530,7 +585,7 @@
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
+        <left style="thick">
           <color indexed="64"/>
         </left>
         <right style="thin">
@@ -548,7 +603,7 @@
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
+        <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="thin">
@@ -761,8 +816,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36B91720-324F-4249-9D87-9FB5088C2BBE}" name="Tabulka2" displayName="Tabulka2" ref="A2:L18" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
-  <autoFilter ref="A2:L18" xr:uid="{36B91720-324F-4249-9D87-9FB5088C2BBE}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36B91720-324F-4249-9D87-9FB5088C2BBE}" name="Tabulka2" displayName="Tabulka2" ref="A2:M18" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+  <autoFilter ref="A2:M18" xr:uid="{36B91720-324F-4249-9D87-9FB5088C2BBE}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -775,20 +830,22 @@
     <filterColumn colId="9" hiddenButton="1"/>
     <filterColumn colId="10" hiddenButton="1"/>
     <filterColumn colId="11" hiddenButton="1"/>
+    <filterColumn colId="12" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{27762300-EECA-4A09-9AD5-9D7512ED754D}" name="dataset" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{9EA2270C-6ACC-46D7-A881-6B3D3528A0D0}" name="metoda" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{AD6F6BE4-255F-44A1-A2C9-E2B8D74F69B3}" name="0.2" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{F5229BB4-A6A7-49F4-A07F-AC8B062971B5}" name="0.3" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{1F19A5EF-E204-4D92-B38D-116E0475765D}" name="0.35" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{98FB4315-9688-46ED-B0EB-08DE5D450D9E}" name="0.4" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{8B790170-1CF7-45F9-968E-81C815D57C56}" name="0.5" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{0F22BD4B-5BC6-4D1B-BEAD-09DC28D16FEC}" name="30%" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{BB95C2BA-9351-414D-B36B-1C64C935E46D}" name="50%" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{065AAAC9-38C5-47B3-B8DB-4AF902DEBA4E}" name="70%" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{40A314C2-A9ED-4C94-AB7F-0B7A07A233F8}" name="90%" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{AACE5453-1EF4-49C9-856C-2E13D93044EA}" name="původní" dataDxfId="0"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{27762300-EECA-4A09-9AD5-9D7512ED754D}" name="dataset" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{9EA2270C-6ACC-46D7-A881-6B3D3528A0D0}" name="metoda" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{AD6F6BE4-255F-44A1-A2C9-E2B8D74F69B3}" name="0.2" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{F5229BB4-A6A7-49F4-A07F-AC8B062971B5}" name="0.3" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{1F19A5EF-E204-4D92-B38D-116E0475765D}" name="0.35" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{98FB4315-9688-46ED-B0EB-08DE5D450D9E}" name="0.4" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{8B790170-1CF7-45F9-968E-81C815D57C56}" name="0.5" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{524875B6-D135-4CDA-8A53-EBD2497EF7A7}" name="3x3 unit" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{0F22BD4B-5BC6-4D1B-BEAD-09DC28D16FEC}" name="30%" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{BB95C2BA-9351-414D-B36B-1C64C935E46D}" name="50%" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{065AAAC9-38C5-47B3-B8DB-4AF902DEBA4E}" name="70%" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{40A314C2-A9ED-4C94-AB7F-0B7A07A233F8}" name="90%" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{AACE5453-1EF4-49C9-856C-2E13D93044EA}" name="původní" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1091,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A18BC53-8D4E-4913-BFBB-2CAE486F5D55}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1104,33 +1161,37 @@
     <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" customWidth="1"/>
     <col min="5" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C1" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="14" t="s">
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="26"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="24"/>
     </row>
-    <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="18" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="10" t="s">
@@ -1142,51 +1203,55 @@
       <c r="F2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="24" t="s">
+      <c r="L2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="27" t="s">
+      <c r="M2" s="25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="17"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="2"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="15"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="28">
+      <c r="K3" s="2"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="26">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="16">
         <v>39</v>
       </c>
       <c r="D4" s="1">
@@ -1198,33 +1263,36 @@
       <c r="F4" s="1">
         <v>32</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="20">
         <v>26</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="33">
+        <v>38</v>
+      </c>
+      <c r="I4" s="16">
         <v>29</v>
-      </c>
-      <c r="I4" s="1">
-        <v>30</v>
       </c>
       <c r="J4" s="1">
         <v>30</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="1">
+        <v>30</v>
+      </c>
+      <c r="L4" s="5">
         <v>29</v>
       </c>
-      <c r="L4" s="28">
+      <c r="M4" s="26">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="16">
         <v>39</v>
       </c>
       <c r="D5" s="1">
@@ -1236,33 +1304,36 @@
       <c r="F5" s="1">
         <v>34</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="20">
         <v>28</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="33">
+        <v>37</v>
+      </c>
+      <c r="I5" s="16">
         <v>31</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>32</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>28</v>
       </c>
-      <c r="K5" s="5">
+      <c r="L5" s="5">
         <v>33</v>
       </c>
-      <c r="L5" s="28">
+      <c r="M5" s="26">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="16">
         <v>41</v>
       </c>
       <c r="D6" s="1">
@@ -1274,51 +1345,55 @@
       <c r="F6" s="1">
         <v>24</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="20">
         <v>23</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="33">
+        <v>37</v>
+      </c>
+      <c r="I6" s="16">
         <v>30</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>31</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <v>34</v>
       </c>
-      <c r="K6" s="5">
+      <c r="L6" s="5">
         <v>27</v>
       </c>
-      <c r="L6" s="28">
+      <c r="M6" s="26">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="17"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="1"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="16"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="28">
+      <c r="K7" s="1"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="26">
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="16">
         <v>192</v>
       </c>
       <c r="D8" s="1">
@@ -1330,33 +1405,36 @@
       <c r="F8" s="1">
         <v>146</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="20">
         <v>121</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="33">
+        <v>151</v>
+      </c>
+      <c r="I8" s="16">
         <v>150</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <v>150</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K8" s="1">
         <v>147</v>
       </c>
-      <c r="K8" s="5">
+      <c r="L8" s="5">
         <v>143</v>
       </c>
-      <c r="L8" s="28">
+      <c r="M8" s="26">
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="16">
         <v>195</v>
       </c>
       <c r="D9" s="1">
@@ -1368,33 +1446,36 @@
       <c r="F9" s="1">
         <v>162</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="20">
         <v>126</v>
       </c>
-      <c r="H9" s="17">
-        <v>150</v>
-      </c>
-      <c r="I9" s="1">
+      <c r="H9" s="33">
+        <v>149</v>
+      </c>
+      <c r="I9" s="16">
         <v>150</v>
       </c>
       <c r="J9" s="1">
         <v>150</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="1">
+        <v>150</v>
+      </c>
+      <c r="L9" s="5">
         <v>146</v>
       </c>
-      <c r="L9" s="28">
+      <c r="M9" s="26">
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="16">
         <v>192</v>
       </c>
       <c r="D10" s="1">
@@ -1406,51 +1487,55 @@
       <c r="F10" s="1">
         <v>139</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="20">
         <v>101</v>
       </c>
-      <c r="H10" s="17">
-        <v>150</v>
-      </c>
-      <c r="I10" s="1">
+      <c r="H10" s="33">
+        <v>152</v>
+      </c>
+      <c r="I10" s="16">
         <v>150</v>
       </c>
       <c r="J10" s="1">
         <v>150</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="1">
+        <v>150</v>
+      </c>
+      <c r="L10" s="5">
         <v>139</v>
       </c>
-      <c r="L10" s="28">
+      <c r="M10" s="26">
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="5"/>
-      <c r="C11" s="17"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="1"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="16"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="28">
+      <c r="K11" s="1"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="26">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="16">
         <v>23</v>
       </c>
       <c r="D12" s="1">
@@ -1462,33 +1547,36 @@
       <c r="F12" s="1">
         <v>18</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="20">
         <v>14</v>
       </c>
-      <c r="H12" s="17">
+      <c r="H12" s="33">
+        <v>26</v>
+      </c>
+      <c r="I12" s="16">
         <v>31</v>
       </c>
-      <c r="I12" s="1">
+      <c r="J12" s="1">
         <v>45</v>
       </c>
-      <c r="J12" s="1">
+      <c r="K12" s="1">
         <v>40</v>
       </c>
-      <c r="K12" s="5">
+      <c r="L12" s="5">
         <v>39</v>
       </c>
-      <c r="L12" s="28">
+      <c r="M12" s="26">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="16">
         <v>25</v>
       </c>
       <c r="D13" s="1">
@@ -1500,33 +1588,36 @@
       <c r="F13" s="1">
         <v>19</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="20">
         <v>17</v>
       </c>
-      <c r="H13" s="17">
+      <c r="H13" s="33">
+        <v>23</v>
+      </c>
+      <c r="I13" s="16">
         <v>26</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="1">
         <v>32</v>
       </c>
-      <c r="J13" s="1">
+      <c r="K13" s="1">
         <v>40</v>
       </c>
-      <c r="K13" s="5">
+      <c r="L13" s="5">
         <v>52</v>
       </c>
-      <c r="L13" s="28">
+      <c r="M13" s="26">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="16">
         <v>27</v>
       </c>
       <c r="D14" s="1">
@@ -1538,51 +1629,55 @@
       <c r="F14" s="1">
         <v>18</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="20">
         <v>14</v>
       </c>
-      <c r="H14" s="17">
+      <c r="H14" s="33">
+        <v>25</v>
+      </c>
+      <c r="I14" s="16">
         <v>27</v>
       </c>
-      <c r="I14" s="1">
+      <c r="J14" s="1">
         <v>34</v>
       </c>
-      <c r="J14" s="1">
+      <c r="K14" s="1">
         <v>43</v>
       </c>
-      <c r="K14" s="5">
+      <c r="L14" s="5">
         <v>52</v>
       </c>
-      <c r="L14" s="28">
+      <c r="M14" s="26">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="17"/>
+      <c r="C15" s="16"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="1"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="16"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="28">
+      <c r="K15" s="1"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="26">
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="16">
         <v>165</v>
       </c>
       <c r="D16" s="1">
@@ -1594,33 +1689,36 @@
       <c r="F16" s="1">
         <v>138</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="20">
         <v>133</v>
       </c>
-      <c r="H16" s="17">
+      <c r="H16" s="33">
+        <v>148</v>
+      </c>
+      <c r="I16" s="16">
         <v>115</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J16" s="1">
         <v>126</v>
       </c>
-      <c r="J16" s="1">
+      <c r="K16" s="1">
         <v>122</v>
       </c>
-      <c r="K16" s="5">
+      <c r="L16" s="5">
         <v>86</v>
       </c>
-      <c r="L16" s="28">
+      <c r="M16" s="26">
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="16">
         <v>175</v>
       </c>
       <c r="D17" s="1">
@@ -1632,33 +1730,36 @@
       <c r="F17" s="1">
         <v>151</v>
       </c>
-      <c r="G17" s="22">
+      <c r="G17" s="20">
         <v>127</v>
       </c>
-      <c r="H17" s="17">
+      <c r="H17" s="33">
+        <v>158</v>
+      </c>
+      <c r="I17" s="16">
         <v>115</v>
       </c>
-      <c r="I17" s="1">
+      <c r="J17" s="1">
         <v>132</v>
       </c>
-      <c r="J17" s="1">
+      <c r="K17" s="1">
         <v>122</v>
       </c>
-      <c r="K17" s="5">
+      <c r="L17" s="5">
         <v>115</v>
       </c>
-      <c r="L17" s="28">
+      <c r="M17" s="26">
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="17">
         <v>144</v>
       </c>
       <c r="D18" s="8">
@@ -1670,28 +1771,31 @@
       <c r="F18" s="8">
         <v>39</v>
       </c>
-      <c r="G18" s="23">
+      <c r="G18" s="21">
         <v>30</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="31">
+        <v>144</v>
+      </c>
+      <c r="I18" s="17">
         <v>125</v>
       </c>
-      <c r="I18" s="8">
+      <c r="J18" s="8">
         <v>128</v>
       </c>
-      <c r="J18" s="8">
+      <c r="K18" s="8">
         <v>109</v>
       </c>
-      <c r="K18" s="9">
+      <c r="L18" s="9">
         <v>95</v>
       </c>
-      <c r="L18" s="29">
+      <c r="M18" s="27">
         <v>112</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="I1:L1"/>
     <mergeCell ref="C1:G1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1704,6 +1808,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100BCBFF2982C0CB045A7EE06C9503D8796" ma:contentTypeVersion="11" ma:contentTypeDescription="Vytvoří nový dokument" ma:contentTypeScope="" ma:versionID="11d6c1f5bf15e06027402a0a733460bf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4323e199-edcb-4945-be5f-cca9371163df" xmlns:ns4="cfa1977f-9b9c-4d3d-b010-b84f5560bd13" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="91941e2baf353d5164072b22045d3f64" ns3:_="" ns4:_="">
     <xsd:import namespace="4323e199-edcb-4945-be5f-cca9371163df"/>
@@ -1912,15 +2025,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1928,6 +2032,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F070C89-41AB-42BF-BF26-4394BF9E3193}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEAFC8AE-4DF9-49A0-8985-3743388CF25F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1942,14 +2054,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F070C89-41AB-42BF-BF26-4394BF9E3193}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
erosion and dilatation fix
</commit_message>
<xml_diff>
--- a/data/vysledky-mazani.xlsx
+++ b/data/vysledky-mazani.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\bakalarska-prace\bakalarska-prace\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AE937D-4D44-445E-BB6B-C951CFC0FE3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB3102A-370A-4F13-8927-E1F8150CAB43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1896" windowWidth="17280" windowHeight="8964" xr2:uid="{3CC789BC-E248-4C1E-B58B-9660197E393A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3CC789BC-E248-4C1E-B58B-9660197E393A}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
   <si>
     <t>dataset</t>
   </si>
@@ -123,6 +123,30 @@
   </si>
   <si>
     <t>3x2 col2</t>
+  </si>
+  <si>
+    <t>3x3 unit4</t>
+  </si>
+  <si>
+    <t>3x3 unit5</t>
+  </si>
+  <si>
+    <t>3x3 col3</t>
+  </si>
+  <si>
+    <t>3x2 col3</t>
+  </si>
+  <si>
+    <t>3x3 col4</t>
+  </si>
+  <si>
+    <t>3x2 col4</t>
+  </si>
+  <si>
+    <t>dilat-eros-eros-dilat</t>
+  </si>
+  <si>
+    <t>eros-dilat-dilat-eros</t>
   </si>
 </sst>
 </file>
@@ -467,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -498,6 +522,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -511,7 +538,63 @@
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="28">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -620,6 +703,34 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -901,8 +1012,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36B91720-324F-4249-9D87-9FB5088C2BBE}" name="Tabulka2" displayName="Tabulka2" ref="A2:R18" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
-  <autoFilter ref="A2:R18" xr:uid="{36B91720-324F-4249-9D87-9FB5088C2BBE}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36B91720-324F-4249-9D87-9FB5088C2BBE}" name="Tabulka2" displayName="Tabulka2" ref="A2:X18" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+  <autoFilter ref="A2:X18" xr:uid="{36B91720-324F-4249-9D87-9FB5088C2BBE}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -921,26 +1032,38 @@
     <filterColumn colId="15" hiddenButton="1"/>
     <filterColumn colId="16" hiddenButton="1"/>
     <filterColumn colId="17" hiddenButton="1"/>
+    <filterColumn colId="18" hiddenButton="1"/>
+    <filterColumn colId="19" hiddenButton="1"/>
+    <filterColumn colId="20" hiddenButton="1"/>
+    <filterColumn colId="21" hiddenButton="1"/>
+    <filterColumn colId="22" hiddenButton="1"/>
+    <filterColumn colId="23" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{27762300-EECA-4A09-9AD5-9D7512ED754D}" name="dataset" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{9EA2270C-6ACC-46D7-A881-6B3D3528A0D0}" name="metoda" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{AD6F6BE4-255F-44A1-A2C9-E2B8D74F69B3}" name="0.2" dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{F5229BB4-A6A7-49F4-A07F-AC8B062971B5}" name="0.3" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{1F19A5EF-E204-4D92-B38D-116E0475765D}" name="0.35" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{98FB4315-9688-46ED-B0EB-08DE5D450D9E}" name="0.4" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{8B790170-1CF7-45F9-968E-81C815D57C56}" name="0.5" dataDxfId="11"/>
-    <tableColumn id="15" xr3:uid="{D9CEDABA-512A-469C-9727-4CAB25112924}" name="3x3 col" dataDxfId="10"/>
-    <tableColumn id="17" xr3:uid="{A0558FA7-C629-4D37-AF8A-5AFA679C3F74}" name="3x2 col" dataDxfId="1"/>
-    <tableColumn id="14" xr3:uid="{4C823DAC-7075-4E01-B708-479BD224C0E8}" name="3x3 unit" dataDxfId="9"/>
-    <tableColumn id="16" xr3:uid="{16FF2237-16D1-487F-A305-73FF73551DCD}" name="3x3 col2" dataDxfId="8"/>
-    <tableColumn id="19" xr3:uid="{61AE01E0-46B1-4BDB-B74F-B23A8F430321}" name="3x2 col2" dataDxfId="0"/>
-    <tableColumn id="13" xr3:uid="{524875B6-D135-4CDA-8A53-EBD2497EF7A7}" name="3x3 unit2" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{0F22BD4B-5BC6-4D1B-BEAD-09DC28D16FEC}" name="30%" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{BB95C2BA-9351-414D-B36B-1C64C935E46D}" name="50%" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{065AAAC9-38C5-47B3-B8DB-4AF902DEBA4E}" name="70%" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{40A314C2-A9ED-4C94-AB7F-0B7A07A233F8}" name="90%" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{AACE5453-1EF4-49C9-856C-2E13D93044EA}" name="původní" dataDxfId="2"/>
+  <tableColumns count="24">
+    <tableColumn id="1" xr3:uid="{27762300-EECA-4A09-9AD5-9D7512ED754D}" name="dataset" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{9EA2270C-6ACC-46D7-A881-6B3D3528A0D0}" name="metoda" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{AD6F6BE4-255F-44A1-A2C9-E2B8D74F69B3}" name="0.2" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{F5229BB4-A6A7-49F4-A07F-AC8B062971B5}" name="0.3" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{1F19A5EF-E204-4D92-B38D-116E0475765D}" name="0.35" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{98FB4315-9688-46ED-B0EB-08DE5D450D9E}" name="0.4" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{8B790170-1CF7-45F9-968E-81C815D57C56}" name="0.5" dataDxfId="17"/>
+    <tableColumn id="15" xr3:uid="{D9CEDABA-512A-469C-9727-4CAB25112924}" name="3x3 col" dataDxfId="16"/>
+    <tableColumn id="17" xr3:uid="{A0558FA7-C629-4D37-AF8A-5AFA679C3F74}" name="3x2 col" dataDxfId="15"/>
+    <tableColumn id="14" xr3:uid="{4C823DAC-7075-4E01-B708-479BD224C0E8}" name="3x3 unit" dataDxfId="14"/>
+    <tableColumn id="16" xr3:uid="{16FF2237-16D1-487F-A305-73FF73551DCD}" name="3x3 col2" dataDxfId="13"/>
+    <tableColumn id="19" xr3:uid="{61AE01E0-46B1-4BDB-B74F-B23A8F430321}" name="3x2 col2" dataDxfId="12"/>
+    <tableColumn id="13" xr3:uid="{524875B6-D135-4CDA-8A53-EBD2497EF7A7}" name="3x3 unit2" dataDxfId="11"/>
+    <tableColumn id="25" xr3:uid="{9F830409-13A2-491C-A58C-E4BEDAD638A7}" name="3x3 col3" dataDxfId="5"/>
+    <tableColumn id="26" xr3:uid="{AD16FDBE-21D5-49C4-97C5-10D228B51BAC}" name="3x2 col3" dataDxfId="4"/>
+    <tableColumn id="27" xr3:uid="{07312A6B-963C-4ABF-ABDE-08597A019F94}" name="3x3 unit5" dataDxfId="3"/>
+    <tableColumn id="28" xr3:uid="{1B8D6485-2B10-4389-9F94-44E973980AB8}" name="3x3 col4" dataDxfId="2"/>
+    <tableColumn id="29" xr3:uid="{614B5C69-EA6C-4F90-8D28-AAFD54379CF2}" name="3x2 col4" dataDxfId="1"/>
+    <tableColumn id="30" xr3:uid="{0C48FFB1-C05C-40F6-BAD2-015512B54526}" name="3x3 unit4" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{0F22BD4B-5BC6-4D1B-BEAD-09DC28D16FEC}" name="30%" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{BB95C2BA-9351-414D-B36B-1C64C935E46D}" name="50%" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{065AAAC9-38C5-47B3-B8DB-4AF902DEBA4E}" name="70%" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{40A314C2-A9ED-4C94-AB7F-0B7A07A233F8}" name="90%" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{AACE5453-1EF4-49C9-856C-2E13D93044EA}" name="původní" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1243,53 +1366,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A18BC53-8D4E-4913-BFBB-2CAE486F5D55}">
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="36.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1"/>
-    <col min="5" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.6640625" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="15.6640625" customWidth="1"/>
-    <col min="13" max="13" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10" customWidth="1"/>
+    <col min="1" max="1" width="10.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="19" width="8.6640625" customWidth="1"/>
+    <col min="20" max="23" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C1" s="30" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C1" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="30" t="s">
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31" t="s">
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="31"/>
-      <c r="M1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="33"/>
       <c r="N1" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="23"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="23"/>
     </row>
-    <row r="2" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1329,23 +1464,41 @@
       <c r="M2" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="T2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="U2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="V2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="21" t="s">
+      <c r="W2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="24" t="s">
+      <c r="X2" s="24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1361,15 +1514,21 @@
       <c r="K3" s="29"/>
       <c r="L3" s="29"/>
       <c r="M3" s="29"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="25">
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="22"/>
+      <c r="X3" s="25">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -1377,55 +1536,67 @@
         <v>3</v>
       </c>
       <c r="C4" s="15">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E4" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="19">
+        <v>25</v>
+      </c>
+      <c r="H4" s="29">
+        <v>35</v>
+      </c>
+      <c r="I4" s="29">
+        <v>28</v>
+      </c>
+      <c r="J4" s="29">
+        <v>38</v>
+      </c>
+      <c r="K4" s="29">
+        <v>33</v>
+      </c>
+      <c r="L4" s="29">
         <v>26</v>
       </c>
-      <c r="H4" s="29">
-        <v>36</v>
-      </c>
-      <c r="I4" s="29">
+      <c r="M4" s="29">
+        <v>40</v>
+      </c>
+      <c r="N4" s="29">
+        <v>38</v>
+      </c>
+      <c r="O4" s="29">
+        <v>30</v>
+      </c>
+      <c r="P4" s="29">
+        <v>38</v>
+      </c>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
+      <c r="T4" s="15">
         <v>29</v>
       </c>
-      <c r="J4" s="29">
-        <v>37</v>
-      </c>
-      <c r="K4" s="29">
-        <v>32</v>
-      </c>
-      <c r="L4" s="29">
+      <c r="U4" s="1">
         <v>30</v>
       </c>
-      <c r="M4" s="29">
-        <v>38</v>
-      </c>
-      <c r="N4" s="15">
+      <c r="V4" s="1">
+        <v>30</v>
+      </c>
+      <c r="W4" s="5">
         <v>29</v>
       </c>
-      <c r="O4" s="1">
+      <c r="X4" s="25">
         <v>30</v>
       </c>
-      <c r="P4" s="1">
-        <v>30</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>29</v>
-      </c>
-      <c r="R4" s="25">
-        <v>30</v>
-      </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1465,23 +1636,29 @@
       <c r="M5" s="29">
         <v>37</v>
       </c>
-      <c r="N5" s="15">
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="15">
         <v>31</v>
       </c>
-      <c r="O5" s="1">
+      <c r="U5" s="1">
         <v>32</v>
       </c>
-      <c r="P5" s="1">
+      <c r="V5" s="1">
         <v>28</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="W5" s="5">
         <v>33</v>
       </c>
-      <c r="R5" s="25">
+      <c r="X5" s="25">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
@@ -1521,23 +1698,29 @@
       <c r="M6" s="29">
         <v>37</v>
       </c>
-      <c r="N6" s="15">
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="15">
         <v>30</v>
       </c>
-      <c r="O6" s="1">
+      <c r="U6" s="1">
         <v>31</v>
       </c>
-      <c r="P6" s="1">
+      <c r="V6" s="1">
         <v>34</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="W6" s="5">
         <v>27</v>
       </c>
-      <c r="R6" s="25">
+      <c r="X6" s="25">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -1553,15 +1736,21 @@
       <c r="K7" s="29"/>
       <c r="L7" s="29"/>
       <c r="M7" s="29"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="25">
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="25">
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -1601,23 +1790,29 @@
       <c r="M8" s="29">
         <v>151</v>
       </c>
-      <c r="N8" s="15">
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="15">
         <v>150</v>
       </c>
-      <c r="O8" s="1">
+      <c r="U8" s="1">
         <v>150</v>
       </c>
-      <c r="P8" s="1">
+      <c r="V8" s="1">
         <v>147</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="W8" s="5">
         <v>143</v>
       </c>
-      <c r="R8" s="25">
+      <c r="X8" s="25">
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -1657,23 +1852,29 @@
       <c r="M9" s="29">
         <v>149</v>
       </c>
-      <c r="N9" s="15">
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="15">
         <v>150</v>
       </c>
-      <c r="O9" s="1">
+      <c r="U9" s="1">
         <v>150</v>
       </c>
-      <c r="P9" s="1">
+      <c r="V9" s="1">
         <v>150</v>
       </c>
-      <c r="Q9" s="5">
+      <c r="W9" s="5">
         <v>146</v>
       </c>
-      <c r="R9" s="25">
+      <c r="X9" s="25">
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
@@ -1713,23 +1914,29 @@
       <c r="M10" s="29">
         <v>152</v>
       </c>
-      <c r="N10" s="15">
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="29"/>
+      <c r="T10" s="15">
         <v>150</v>
       </c>
-      <c r="O10" s="1">
+      <c r="U10" s="1">
         <v>150</v>
       </c>
-      <c r="P10" s="1">
+      <c r="V10" s="1">
         <v>150</v>
       </c>
-      <c r="Q10" s="5">
+      <c r="W10" s="5">
         <v>139</v>
       </c>
-      <c r="R10" s="25">
+      <c r="X10" s="25">
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1745,15 +1952,21 @@
       <c r="K11" s="29"/>
       <c r="L11" s="29"/>
       <c r="M11" s="29"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="25">
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="29"/>
+      <c r="R11" s="29"/>
+      <c r="S11" s="29"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="25">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
@@ -1793,23 +2006,29 @@
       <c r="M12" s="29">
         <v>26</v>
       </c>
-      <c r="N12" s="15">
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="29"/>
+      <c r="S12" s="29"/>
+      <c r="T12" s="15">
         <v>31</v>
       </c>
-      <c r="O12" s="1">
+      <c r="U12" s="1">
         <v>45</v>
       </c>
-      <c r="P12" s="1">
+      <c r="V12" s="1">
         <v>40</v>
       </c>
-      <c r="Q12" s="5">
+      <c r="W12" s="5">
         <v>39</v>
       </c>
-      <c r="R12" s="25">
+      <c r="X12" s="25">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -1849,23 +2068,29 @@
       <c r="M13" s="29">
         <v>23</v>
       </c>
-      <c r="N13" s="15">
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="29"/>
+      <c r="R13" s="29"/>
+      <c r="S13" s="29"/>
+      <c r="T13" s="15">
         <v>26</v>
       </c>
-      <c r="O13" s="1">
+      <c r="U13" s="1">
         <v>32</v>
       </c>
-      <c r="P13" s="1">
+      <c r="V13" s="1">
         <v>40</v>
       </c>
-      <c r="Q13" s="5">
+      <c r="W13" s="5">
         <v>52</v>
       </c>
-      <c r="R13" s="25">
+      <c r="X13" s="25">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1905,23 +2130,29 @@
       <c r="M14" s="29">
         <v>25</v>
       </c>
-      <c r="N14" s="15">
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="29"/>
+      <c r="R14" s="29"/>
+      <c r="S14" s="29"/>
+      <c r="T14" s="15">
         <v>27</v>
       </c>
-      <c r="O14" s="1">
+      <c r="U14" s="1">
         <v>34</v>
       </c>
-      <c r="P14" s="1">
+      <c r="V14" s="1">
         <v>43</v>
       </c>
-      <c r="Q14" s="5">
+      <c r="W14" s="5">
         <v>52</v>
       </c>
-      <c r="R14" s="25">
+      <c r="X14" s="25">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
@@ -1937,15 +2168,21 @@
       <c r="K15" s="29"/>
       <c r="L15" s="29"/>
       <c r="M15" s="29"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="25">
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="29"/>
+      <c r="R15" s="29"/>
+      <c r="S15" s="29"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="25">
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
@@ -1985,23 +2222,29 @@
       <c r="M16" s="29">
         <v>148</v>
       </c>
-      <c r="N16" s="15">
+      <c r="N16" s="29"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="29"/>
+      <c r="Q16" s="29"/>
+      <c r="R16" s="29"/>
+      <c r="S16" s="29"/>
+      <c r="T16" s="15">
         <v>115</v>
       </c>
-      <c r="O16" s="1">
+      <c r="U16" s="1">
         <v>126</v>
       </c>
-      <c r="P16" s="1">
+      <c r="V16" s="1">
         <v>122</v>
       </c>
-      <c r="Q16" s="5">
+      <c r="W16" s="5">
         <v>86</v>
       </c>
-      <c r="R16" s="25">
+      <c r="X16" s="25">
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>8</v>
       </c>
@@ -2041,23 +2284,29 @@
       <c r="M17" s="29">
         <v>158</v>
       </c>
-      <c r="N17" s="15">
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="29"/>
+      <c r="S17" s="29"/>
+      <c r="T17" s="15">
         <v>115</v>
       </c>
-      <c r="O17" s="1">
+      <c r="U17" s="1">
         <v>132</v>
       </c>
-      <c r="P17" s="1">
+      <c r="V17" s="1">
         <v>122</v>
       </c>
-      <c r="Q17" s="5">
+      <c r="W17" s="5">
         <v>115</v>
       </c>
-      <c r="R17" s="25">
+      <c r="X17" s="25">
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>8</v>
       </c>
@@ -2097,25 +2346,31 @@
       <c r="M18" s="27">
         <v>144</v>
       </c>
-      <c r="N18" s="16">
+      <c r="N18" s="27"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="27"/>
+      <c r="R18" s="27"/>
+      <c r="S18" s="27"/>
+      <c r="T18" s="16">
         <v>125</v>
       </c>
-      <c r="O18" s="8">
+      <c r="U18" s="8">
         <v>128</v>
       </c>
-      <c r="P18" s="8">
+      <c r="V18" s="8">
         <v>109</v>
       </c>
-      <c r="Q18" s="9">
+      <c r="W18" s="9">
         <v>95</v>
       </c>
-      <c r="R18" s="26">
+      <c r="X18" s="26">
         <v>112</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="T1:W1"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
@@ -2130,15 +2385,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100BCBFF2982C0CB045A7EE06C9503D8796" ma:contentTypeVersion="11" ma:contentTypeDescription="Vytvoří nový dokument" ma:contentTypeScope="" ma:versionID="11d6c1f5bf15e06027402a0a733460bf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4323e199-edcb-4945-be5f-cca9371163df" xmlns:ns4="cfa1977f-9b9c-4d3d-b010-b84f5560bd13" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="91941e2baf353d5164072b22045d3f64" ns3:_="" ns4:_="">
     <xsd:import namespace="4323e199-edcb-4945-be5f-cca9371163df"/>
@@ -2347,6 +2593,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2354,14 +2609,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F070C89-41AB-42BF-BF26-4394BF9E3193}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEAFC8AE-4DF9-49A0-8985-3743388CF25F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2376,6 +2623,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F070C89-41AB-42BF-BF26-4394BF9E3193}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>